<commit_message>
update formate template alumni
</commit_message>
<xml_diff>
--- a/public/Format Alumni.xlsx
+++ b/public/Format Alumni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\TS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7CCF0B-8116-4422-B76B-221B31B48C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455ECE68-C9D8-432A-AF03-80D6EF6E6068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,16 +39,16 @@
     <t>NIM</t>
   </si>
   <si>
-    <t>Nama</t>
+    <t>Email</t>
   </si>
   <si>
-    <t>Program Studi</t>
+    <t>Study Program</t>
   </si>
   <si>
-    <t>Tanggal Lulus</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>Email</t>
+    <t>Date Passed</t>
   </si>
 </sst>
 </file>
@@ -336,7 +336,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -356,13 +356,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
       </c>
       <c r="F1" s="2"/>
     </row>

</xml_diff>

<commit_message>
fixing format excel for import data alumni
</commit_message>
<xml_diff>
--- a/public/Format Alumni.xlsx
+++ b/public/Format Alumni.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\TS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455ECE68-C9D8-432A-AF03-80D6EF6E6068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC35BB27-2FC0-41DA-A31B-2F204BBD6755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -336,7 +336,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -344,8 +344,8 @@
     <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.109375" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="25.77734375" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -359,10 +359,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F1" s="2"/>
     </row>

</xml_diff>